<commit_message>
inport tll + minor update
</commit_message>
<xml_diff>
--- a/Data/EXCEL/excel_PoC.xlsx
+++ b/Data/EXCEL/excel_PoC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaras\Documents\GitHub\PPtology\Data\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D83C98-5765-4BE6-A604-73FD173206B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8128E1-A19B-4249-9562-4A07009C3831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>nodes</t>
   </si>
@@ -37,12 +37,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>edges</t>
-  </si>
-  <si>
     <t>from</t>
   </si>
   <si>
@@ -74,17 +68,166 @@
   </si>
   <si>
     <t>PoC Feedwater pump</t>
+  </si>
+  <si>
+    <t>N052271</t>
+  </si>
+  <si>
+    <t>PP description</t>
+  </si>
+  <si>
+    <t>Device description</t>
+  </si>
+  <si>
+    <t>261</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>501</t>
+  </si>
+  <si>
+    <t>561</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>538</t>
+  </si>
+  <si>
+    <t>386.46</t>
+  </si>
+  <si>
+    <t>pipe_id</t>
+  </si>
+  <si>
+    <t>pipe_261_176</t>
+  </si>
+  <si>
+    <t>pipe_176_501</t>
+  </si>
+  <si>
+    <t>pipe_501_561</t>
+  </si>
+  <si>
+    <t>pipe_561_261</t>
+  </si>
+  <si>
+    <t>state_id</t>
+  </si>
+  <si>
+    <t>pressure_id</t>
+  </si>
+  <si>
+    <t>temp_id</t>
+  </si>
+  <si>
+    <t>massflow_id</t>
+  </si>
+  <si>
+    <t>Case_id</t>
+  </si>
+  <si>
+    <t>N052271_1</t>
+  </si>
+  <si>
+    <t>st_N052271-1_261_176</t>
+  </si>
+  <si>
+    <t>st_N052271-1_176_501</t>
+  </si>
+  <si>
+    <t>st_N052271-1_501_561</t>
+  </si>
+  <si>
+    <t>st_N052271-1_561_261</t>
+  </si>
+  <si>
+    <t>p_N052271-1_261_177</t>
+  </si>
+  <si>
+    <t>p_N052271-1_176_502</t>
+  </si>
+  <si>
+    <t>p_N052271-1_501_562</t>
+  </si>
+  <si>
+    <t>p_N052271-1_561_262</t>
+  </si>
+  <si>
+    <t>t_N052271-1_261_178</t>
+  </si>
+  <si>
+    <t>t_N052271-1_176_503</t>
+  </si>
+  <si>
+    <t>t_N052271-1_501_563</t>
+  </si>
+  <si>
+    <t>t_N052271-1_561_263</t>
+  </si>
+  <si>
+    <t>mf_N052271-1_261_179</t>
+  </si>
+  <si>
+    <t>mf_N052271-1_176_504</t>
+  </si>
+  <si>
+    <t>mf_N052271-1_501_564</t>
+  </si>
+  <si>
+    <t>mf_N052271-1_561_264</t>
+  </si>
+  <si>
+    <t>pipe_in_case</t>
+  </si>
+  <si>
+    <t>N052271_1_pipe_261_176</t>
+  </si>
+  <si>
+    <t>N052271_1_pipe_176_501</t>
+  </si>
+  <si>
+    <t>N052271_1_pipe_501_561</t>
+  </si>
+  <si>
+    <t>N052271_1_pipe_561_261</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#.0"/>
-    <numFmt numFmtId="165" formatCode="0.##"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -103,6 +246,12 @@
     <font>
       <sz val="10"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -146,22 +295,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -425,108 +569,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>261</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3">
-        <v>176</v>
-      </c>
-      <c r="C4" s="3">
-        <v>118</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>501</v>
-      </c>
-      <c r="C5">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3">
-        <v>561</v>
-      </c>
-      <c r="C6" s="3">
-        <v>70</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1048576" ht="13.2" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="1048576" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -534,118 +695,232 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:L1048575"/>
   <sheetViews>
-    <sheetView zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>261</v>
-      </c>
-      <c r="B3">
-        <v>176</v>
-      </c>
-      <c r="C3" s="5">
-        <v>92</v>
-      </c>
-      <c r="D3" s="5">
-        <v>538</v>
-      </c>
-      <c r="E3">
-        <v>386.46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>176</v>
-      </c>
-      <c r="B4" s="3">
-        <v>501</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="D4" s="7">
-        <v>94</v>
-      </c>
-      <c r="E4" s="3">
-        <v>386.46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>501</v>
-      </c>
-      <c r="B5">
-        <v>561</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0.85</v>
-      </c>
-      <c r="D5" s="5">
+    </row>
+    <row r="2" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="E5">
-        <v>386.46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>561</v>
-      </c>
-      <c r="B6" s="3">
-        <v>261</v>
-      </c>
-      <c r="C6" s="7">
-        <v>120</v>
-      </c>
-      <c r="D6" s="7">
-        <v>90</v>
-      </c>
-      <c r="E6" s="3">
-        <v>386.46</v>
-      </c>
-    </row>
-    <row r="1048576" ht="13.2" x14ac:dyDescent="0.25"/>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="1048575" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>